<commit_message>
Updated Cose of Food and HH outliers
</commit_message>
<xml_diff>
--- a/2progs/RestrictedVariablesSet.xlsx
+++ b/2progs/RestrictedVariablesSet.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/colleenodonnell/Box Sync/KenyaPovertyTargetingModel/2progs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fernandoguzman/Box/KenyaPovertyTargetingModel/2progs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89EEDBD3-A32F-524F-B2C8-EF90CCBF5D86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A07E3FDB-174C-3C40-BE0A-B73437354B7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14820" xr2:uid="{3D3654ED-EF38-9C41-8864-343C92206527}"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14820" activeTab="1" xr2:uid="{3D3654ED-EF38-9C41-8864-343C92206527}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Household &amp; Food" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,16 +35,109 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Variable Name</t>
+  </si>
+  <si>
+    <t>number_dwellings</t>
+  </si>
+  <si>
+    <t>number_habitablerooms</t>
+  </si>
+  <si>
+    <t>floor_material</t>
+  </si>
+  <si>
+    <t>roof_material</t>
+  </si>
+  <si>
+    <t>wall_material</t>
+  </si>
+  <si>
+    <t>toilet_type</t>
+  </si>
+  <si>
+    <t>share_toilet</t>
+  </si>
+  <si>
+    <t>lighting_source</t>
+  </si>
+  <si>
+    <t>own_radio</t>
+  </si>
+  <si>
+    <t>own_television</t>
+  </si>
+  <si>
+    <t>own_satelitedish</t>
+  </si>
+  <si>
+    <t>own_smartphone</t>
+  </si>
+  <si>
+    <t>own_refrigerator</t>
+  </si>
+  <si>
+    <t>own_table</t>
+  </si>
+  <si>
+    <t>own_bed</t>
+  </si>
+  <si>
+    <t>own_mattress</t>
+  </si>
+  <si>
+    <t>own_mosquitonet</t>
+  </si>
+  <si>
+    <t>own_fan</t>
+  </si>
+  <si>
+    <t>own_bicycle</t>
+  </si>
+  <si>
+    <t>own_motorcycle</t>
+  </si>
+  <si>
+    <t>own_car</t>
+  </si>
+  <si>
+    <t>own_generator</t>
+  </si>
+  <si>
+    <t>own_solarpanels</t>
+  </si>
+  <si>
+    <t>own_kerosenestove</t>
+  </si>
+  <si>
+    <t>own_charcoaljiko</t>
+  </si>
+  <si>
+    <t>own_wheelbarrow</t>
+  </si>
+  <si>
+    <t>own_ironfencing</t>
+  </si>
+  <si>
+    <t>own_farmanimals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Food Variable Name </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Household Variable Name </t>
+  </si>
+  <si>
+    <t>hh_purchasedfood7d</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -51,13 +145,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -72,8 +180,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -390,7 +499,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{762F8EB9-90A6-BC43-94FF-58FCD3315797}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="112" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -407,4 +516,174 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20FCEE02-590A-F94F-B770-3BB87D0648AD}">
+  <dimension ref="A1:C29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.1640625" customWidth="1"/>
+    <col min="3" max="3" width="18.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>